<commit_message>
Atualização dos endereços no import-2.xlsx
</commit_message>
<xml_diff>
--- a/import-2.xlsx
+++ b/import-2.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">contato@silva.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua Jaragua;1000;75100100;Distrito Industrial;Anápolis;GO</t>
+    <t xml:space="preserve">Avenida do estado;1000;01025020;Centro;São Paulo;SP</t>
   </si>
   <si>
     <t xml:space="preserve">17.830.029/0001-01</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">adm@costa-trans.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua sei la;1000;75100100;Distrito Industrial;Anápolis;GO</t>
+    <t xml:space="preserve">Avenida Antártica;s/n;05003020;Água Branca;São Paulo;SP</t>
   </si>
   <si>
     <t xml:space="preserve">05.555.382/0001-33</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">compras@diasalim.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua suspeita;1000;75100100;Distrito Industrial;Anápolis;GO</t>
+    <t xml:space="preserve">Estrada do carrapicho;4;05275015;Anhanguera;São Paulo;SP</t>
   </si>
   <si>
     <t xml:space="preserve">15.415.777/0001-94</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">financeiro@moreira.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua das garças;1000;75100100;Distrito Industrial;Anápolis;GO</t>
+    <t xml:space="preserve">Rua Ágatha Cristie;10;04875160;Chácara Santo Amaro;São Paulo;SP</t>
   </si>
   <si>
     <t xml:space="preserve">05742607000160</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">consultoria@fe.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua janeiros;1000;75100100;Distrito Industrial;Anápolis;GO</t>
+    <t xml:space="preserve">Rua janeiros;1000;04116000;Jardim Vila Mariana;São Paulo;SP</t>
   </si>
 </sst>
 </file>
@@ -227,36 +227,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -513,216 +509,216 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="47.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="47.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="1" t="n">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="n">
         <v>75071695</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5" t="n">
+      <c r="G2" s="2"/>
+      <c r="H2" s="4" t="n">
         <v>36765</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="1" t="n">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="n">
         <v>987654321</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5" t="n">
+      <c r="H3" s="2"/>
+      <c r="I3" s="4" t="n">
         <v>40188</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="1" t="n">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="n">
         <v>123456789</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5" t="n">
+      <c r="H4" s="2"/>
+      <c r="I4" s="4" t="n">
         <v>42068</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="1" t="n">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="n">
         <v>321654987</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5" t="n">
+      <c r="H5" s="2"/>
+      <c r="I5" s="4" t="n">
         <v>38515</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="1" t="n">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="n">
         <v>456123789</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5" t="n">
+      <c r="H6" s="2"/>
+      <c r="I6" s="4" t="n">
         <v>43365</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="1" t="n">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="n">
         <v>789123456</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5" t="n">
+      <c r="H7" s="2"/>
+      <c r="I7" s="4" t="n">
         <v>43939</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="2" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>